<commit_message>
My hands are typing words
</commit_message>
<xml_diff>
--- a/production/manual_bom/bom.xlsx
+++ b/production/manual_bom/bom.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\krist\Documents\beetle_boards\tiny-scarab\production\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\krist\Documents\beetle_boards\tiny-scarab\production\manual_bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE9628F1-B996-42FB-8A3F-E806AC5F5CCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1009D36-59C3-4627-A0A3-53B1B659311D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="0" windowWidth="19380" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="ExternalData_1" localSheetId="0" hidden="1">bom!$A$1:$P$38</definedName>
+    <definedName name="ExternalData_1" localSheetId="0" hidden="1">bom!$A$1:$Q$38</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="206">
   <si>
     <t>Item</t>
   </si>
@@ -659,16 +659,22 @@
     <t>Ordered</t>
   </si>
   <si>
-    <t>Lead Time</t>
-  </si>
-  <si>
     <t>Extra order</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Total Price Per Board</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="0.000000"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -708,12 +714,18 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="11">
+    <dxf>
+      <numFmt numFmtId="168" formatCode="0.000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="0.000000"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -756,8 +768,8 @@
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExternalData_1" connectionId="1" xr16:uid="{2721C712-E83D-41AB-96AA-43CA19B521F0}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh nextId="25">
-    <queryTableFields count="16">
+  <queryTableRefresh nextId="26">
+    <queryTableFields count="17">
       <queryTableField id="1" name="Item" tableColumnId="1"/>
       <queryTableField id="2" name="Qty" tableColumnId="2"/>
       <queryTableField id="3" name="Reference(s)" tableColumnId="3"/>
@@ -769,6 +781,7 @@
       <queryTableField id="22" dataBound="0" tableColumnId="7"/>
       <queryTableField id="24" dataBound="0" tableColumnId="5"/>
       <queryTableField id="23" dataBound="0" tableColumnId="8"/>
+      <queryTableField id="25" dataBound="0" tableColumnId="17"/>
       <queryTableField id="9" name="AliExpress" tableColumnId="9"/>
       <queryTableField id="10" name="Comment" tableColumnId="10"/>
       <queryTableField id="11" name="DigiKey" tableColumnId="11"/>
@@ -786,27 +799,30 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5230B8D1-99E5-4459-BFDF-8FD98159B394}" name="bom" displayName="bom" ref="A1:P38" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:P38" xr:uid="{5230B8D1-99E5-4459-BFDF-8FD98159B394}"/>
-  <tableColumns count="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5230B8D1-99E5-4459-BFDF-8FD98159B394}" name="bom" displayName="bom" ref="A1:Q38" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:Q38" xr:uid="{5230B8D1-99E5-4459-BFDF-8FD98159B394}"/>
+  <tableColumns count="17">
     <tableColumn id="1" xr3:uid="{FE9C4D66-9E81-4CFB-8A09-A00B62AC3F27}" uniqueName="1" name="Item" queryTableFieldId="1"/>
     <tableColumn id="2" xr3:uid="{60ACA556-DAAA-43F7-9430-676EA843F6DC}" uniqueName="2" name="Qty" queryTableFieldId="2"/>
-    <tableColumn id="3" xr3:uid="{B0C27889-558E-43B3-BB52-1C17E20D77F7}" uniqueName="3" name="Reference(s)" queryTableFieldId="3" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{490D85B1-6ECD-4AEA-B64D-1AFBF8637BCC}" uniqueName="4" name="Value" queryTableFieldId="4" dataDxfId="7"/>
-    <tableColumn id="15" xr3:uid="{4CE4FA41-799A-42FD-944F-88C38C8E855B}" uniqueName="15" name="Manufacturer" queryTableFieldId="15" dataDxfId="6"/>
-    <tableColumn id="14" xr3:uid="{22938EE0-2990-4607-B043-FF178F1C63F5}" uniqueName="14" name="MPN" queryTableFieldId="14" dataDxfId="5"/>
-    <tableColumn id="13" xr3:uid="{709C57DE-9E94-44F2-9904-930C4B22DF02}" uniqueName="13" name="JLCPCB Part #" queryTableFieldId="13" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{3610E293-B6EA-45AC-9D53-33E203A1D09D}" uniqueName="6" name="Needed" queryTableFieldId="21" dataDxfId="3">
+    <tableColumn id="3" xr3:uid="{B0C27889-558E-43B3-BB52-1C17E20D77F7}" uniqueName="3" name="Reference(s)" queryTableFieldId="3" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{490D85B1-6ECD-4AEA-B64D-1AFBF8637BCC}" uniqueName="4" name="Value" queryTableFieldId="4" dataDxfId="9"/>
+    <tableColumn id="15" xr3:uid="{4CE4FA41-799A-42FD-944F-88C38C8E855B}" uniqueName="15" name="Manufacturer" queryTableFieldId="15" dataDxfId="8"/>
+    <tableColumn id="14" xr3:uid="{22938EE0-2990-4607-B043-FF178F1C63F5}" uniqueName="14" name="MPN" queryTableFieldId="14" dataDxfId="7"/>
+    <tableColumn id="13" xr3:uid="{709C57DE-9E94-44F2-9904-930C4B22DF02}" uniqueName="13" name="JLCPCB Part #" queryTableFieldId="13" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{3610E293-B6EA-45AC-9D53-33E203A1D09D}" uniqueName="6" name="Needed" queryTableFieldId="21" dataDxfId="5">
       <calculatedColumnFormula>50*bom[[#This Row],[Qty]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="7" xr3:uid="{0AC43B65-BCE0-48A6-AFED-BE6BFCBF0CDC}" uniqueName="7" name="Ordered" queryTableFieldId="22"/>
     <tableColumn id="5" xr3:uid="{6DBB5AA5-41E7-4024-B221-F4A9A52D7420}" uniqueName="5" name="Extra order" queryTableFieldId="24"/>
-    <tableColumn id="8" xr3:uid="{87B515EF-77DF-474C-A454-7D47EBF5667C}" uniqueName="8" name="Lead Time" queryTableFieldId="23"/>
+    <tableColumn id="8" xr3:uid="{87B515EF-77DF-474C-A454-7D47EBF5667C}" uniqueName="8" name="Price" queryTableFieldId="23" dataDxfId="1"/>
+    <tableColumn id="17" xr3:uid="{63C171B3-3B70-4C84-AAE6-2D5E5EB6828A}" uniqueName="17" name="Total Price Per Board" queryTableFieldId="25" dataDxfId="0">
+      <calculatedColumnFormula>bom[[#This Row],[Qty]]*bom[[#This Row],[Price]]</calculatedColumnFormula>
+    </tableColumn>
     <tableColumn id="9" xr3:uid="{F3B8890B-9116-4A6E-9C97-5668BEE4516B}" uniqueName="9" name="AliExpress" queryTableFieldId="9"/>
-    <tableColumn id="10" xr3:uid="{21838332-5814-4455-8CD6-846F33D528F2}" uniqueName="10" name="Comment" queryTableFieldId="10" dataDxfId="2"/>
-    <tableColumn id="11" xr3:uid="{98085884-14DA-409E-8493-738F552FC7D2}" uniqueName="11" name="DigiKey" queryTableFieldId="11" dataDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{21838332-5814-4455-8CD6-846F33D528F2}" uniqueName="10" name="Comment" queryTableFieldId="10" dataDxfId="4"/>
+    <tableColumn id="11" xr3:uid="{98085884-14DA-409E-8493-738F552FC7D2}" uniqueName="11" name="DigiKey" queryTableFieldId="11" dataDxfId="3"/>
     <tableColumn id="12" xr3:uid="{4912BD51-58E0-4BC5-B9BD-FF51047F4AF6}" uniqueName="12" name="Farnell" queryTableFieldId="12"/>
-    <tableColumn id="16" xr3:uid="{76C67EFC-F0D6-496D-84A8-D41AE352AC19}" uniqueName="16" name="Mouser" queryTableFieldId="16" dataDxfId="0"/>
+    <tableColumn id="16" xr3:uid="{76C67EFC-F0D6-496D-84A8-D41AE352AC19}" uniqueName="16" name="Mouser" queryTableFieldId="16" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1075,10 +1091,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98630DD5-670D-474C-898C-4815DC4C2BE2}">
-  <dimension ref="A1:P38"/>
+  <dimension ref="A1:Q38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E10" workbookViewId="0">
-      <selection activeCell="L43" sqref="L43"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1090,17 +1106,19 @@
     <col min="5" max="5" width="37.7265625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.7265625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
-    <col min="8" max="11" width="15" customWidth="1"/>
-    <col min="12" max="12" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="23.7265625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="30.26953125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="23.453125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="35.453125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="22.26953125" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="15" customWidth="1"/>
+    <col min="11" max="11" width="15" style="2" customWidth="1"/>
+    <col min="12" max="12" width="20.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="23.7265625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="30.26953125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="23.453125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="35.453125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="22.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1129,28 +1147,31 @@
         <v>202</v>
       </c>
       <c r="J1" t="s">
+        <v>203</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="K1" t="s">
-        <v>203</v>
-      </c>
-      <c r="L1" t="s">
+      <c r="L1" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="M1" t="s">
         <v>4</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>5</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>6</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>7</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1179,17 +1200,24 @@
       <c r="I2">
         <v>2400</v>
       </c>
-      <c r="M2" t="s">
+      <c r="K2" s="2">
+        <v>4.4999999999999997E-3</v>
+      </c>
+      <c r="L2" s="2">
+        <f>bom[[#This Row],[Qty]]*bom[[#This Row],[Price]]</f>
+        <v>0.10799999999999998</v>
+      </c>
+      <c r="N2" t="s">
         <v>15</v>
       </c>
-      <c r="N2" t="s">
-        <v>14</v>
-      </c>
-      <c r="P2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="O2" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1218,17 +1246,24 @@
       <c r="I3">
         <v>900</v>
       </c>
-      <c r="M3" t="s">
+      <c r="K3" s="2">
+        <v>8.0999999999999996E-3</v>
+      </c>
+      <c r="L3" s="2">
+        <f>bom[[#This Row],[Qty]]*bom[[#This Row],[Price]]</f>
+        <v>7.2899999999999993E-2</v>
+      </c>
+      <c r="N3" t="s">
         <v>21</v>
       </c>
-      <c r="N3" t="s">
-        <v>14</v>
-      </c>
-      <c r="P3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="O3" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1257,17 +1292,24 @@
       <c r="I4">
         <v>400</v>
       </c>
-      <c r="M4" t="s">
+      <c r="K4" s="2">
+        <v>3.5999999999999999E-3</v>
+      </c>
+      <c r="L4" s="2">
+        <f>bom[[#This Row],[Qty]]*bom[[#This Row],[Price]]</f>
+        <v>1.44E-2</v>
+      </c>
+      <c r="N4" t="s">
         <v>26</v>
       </c>
-      <c r="N4" t="s">
-        <v>14</v>
-      </c>
-      <c r="P4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="O4" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1296,17 +1338,24 @@
       <c r="I5">
         <v>200</v>
       </c>
-      <c r="M5" t="s">
+      <c r="K5" s="2">
+        <v>4.7000000000000002E-3</v>
+      </c>
+      <c r="L5" s="2">
+        <f>bom[[#This Row],[Qty]]*bom[[#This Row],[Price]]</f>
+        <v>9.4000000000000004E-3</v>
+      </c>
+      <c r="N5" t="s">
         <v>30</v>
       </c>
-      <c r="N5" t="s">
-        <v>14</v>
-      </c>
-      <c r="P5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="O5" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1335,17 +1384,24 @@
       <c r="I6">
         <v>400</v>
       </c>
-      <c r="M6" t="s">
+      <c r="K6" s="2">
+        <v>8.9999999999999998E-4</v>
+      </c>
+      <c r="L6" s="2">
+        <f>bom[[#This Row],[Qty]]*bom[[#This Row],[Price]]</f>
+        <v>3.5999999999999999E-3</v>
+      </c>
+      <c r="N6" t="s">
         <v>36</v>
       </c>
-      <c r="N6" t="s">
-        <v>14</v>
-      </c>
-      <c r="P6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="O6" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1374,17 +1430,24 @@
       <c r="I7">
         <v>200</v>
       </c>
-      <c r="M7" t="s">
-        <v>14</v>
+      <c r="K7" s="2">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="L7" s="2">
+        <f>bom[[#This Row],[Qty]]*bom[[#This Row],[Price]]</f>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="N7" t="s">
+        <v>14</v>
+      </c>
+      <c r="O7" t="s">
         <v>42</v>
       </c>
-      <c r="P7" t="s">
+      <c r="Q7" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1413,20 +1476,27 @@
       <c r="I8">
         <v>100</v>
       </c>
-      <c r="M8" t="s">
-        <v>14</v>
+      <c r="K8" s="2">
+        <v>1.6400000000000001E-2</v>
+      </c>
+      <c r="L8" s="2">
+        <f>bom[[#This Row],[Qty]]*bom[[#This Row],[Price]]</f>
+        <v>1.6400000000000001E-2</v>
       </c>
       <c r="N8" t="s">
+        <v>14</v>
+      </c>
+      <c r="O8" t="s">
         <v>49</v>
       </c>
-      <c r="O8">
+      <c r="P8">
         <v>2393466</v>
       </c>
-      <c r="P8" t="s">
+      <c r="Q8" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1455,20 +1525,27 @@
       <c r="I9">
         <v>100</v>
       </c>
-      <c r="M9" t="s">
-        <v>14</v>
+      <c r="K9" s="2">
+        <v>8.6599999999999996E-2</v>
+      </c>
+      <c r="L9" s="2">
+        <f>bom[[#This Row],[Qty]]*bom[[#This Row],[Price]]</f>
+        <v>8.6599999999999996E-2</v>
       </c>
       <c r="N9" t="s">
+        <v>14</v>
+      </c>
+      <c r="O9" t="s">
         <v>56</v>
       </c>
-      <c r="O9">
+      <c r="P9">
         <v>4247180</v>
       </c>
-      <c r="P9" t="s">
+      <c r="Q9" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1497,17 +1574,24 @@
       <c r="I10">
         <v>100</v>
       </c>
-      <c r="M10" t="s">
-        <v>14</v>
+      <c r="K10" s="2">
+        <v>3.78E-2</v>
+      </c>
+      <c r="L10" s="2">
+        <f>bom[[#This Row],[Qty]]*bom[[#This Row],[Price]]</f>
+        <v>3.78E-2</v>
       </c>
       <c r="N10" t="s">
         <v>14</v>
       </c>
-      <c r="P10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="O10" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1536,17 +1620,24 @@
       <c r="I11">
         <v>200</v>
       </c>
-      <c r="M11" t="s">
-        <v>14</v>
+      <c r="K11" s="2">
+        <v>4.82E-2</v>
+      </c>
+      <c r="L11" s="2">
+        <f>bom[[#This Row],[Qty]]*bom[[#This Row],[Price]]</f>
+        <v>9.64E-2</v>
       </c>
       <c r="N11" t="s">
         <v>14</v>
       </c>
-      <c r="P11" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="O11" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1579,22 +1670,26 @@
         <v>100</v>
       </c>
       <c r="K12" s="2">
-        <v>45347</v>
-      </c>
-      <c r="M12" t="s">
-        <v>14</v>
+        <v>0.32090000000000002</v>
+      </c>
+      <c r="L12" s="2">
+        <f>bom[[#This Row],[Qty]]*bom[[#This Row],[Price]]</f>
+        <v>0.64180000000000004</v>
       </c>
       <c r="N12" t="s">
+        <v>14</v>
+      </c>
+      <c r="O12" t="s">
         <v>72</v>
       </c>
-      <c r="O12">
+      <c r="P12">
         <v>4129807</v>
       </c>
-      <c r="P12" t="s">
+      <c r="Q12" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1627,22 +1722,26 @@
         <v>50</v>
       </c>
       <c r="K13" s="2">
-        <v>45347</v>
-      </c>
-      <c r="M13" t="s">
-        <v>14</v>
+        <v>0.3982</v>
+      </c>
+      <c r="L13" s="2">
+        <f>bom[[#This Row],[Qty]]*bom[[#This Row],[Price]]</f>
+        <v>0.3982</v>
       </c>
       <c r="N13" t="s">
+        <v>14</v>
+      </c>
+      <c r="O13" t="s">
         <v>79</v>
       </c>
-      <c r="O13">
+      <c r="P13">
         <v>3954422</v>
       </c>
-      <c r="P13" t="s">
+      <c r="Q13" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1675,22 +1774,26 @@
         <v>100</v>
       </c>
       <c r="K14" s="2">
-        <v>45347</v>
-      </c>
-      <c r="M14" t="s">
-        <v>14</v>
+        <v>0.53139999999999998</v>
+      </c>
+      <c r="L14" s="2">
+        <f>bom[[#This Row],[Qty]]*bom[[#This Row],[Price]]</f>
+        <v>1.0628</v>
       </c>
       <c r="N14" t="s">
+        <v>14</v>
+      </c>
+      <c r="O14" t="s">
         <v>85</v>
       </c>
-      <c r="O14">
+      <c r="P14">
         <v>3954417</v>
       </c>
-      <c r="P14" t="s">
+      <c r="Q14" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1719,20 +1822,27 @@
       <c r="I15">
         <v>600</v>
       </c>
-      <c r="M15" t="s">
-        <v>14</v>
+      <c r="K15" s="2">
+        <v>1.77E-2</v>
+      </c>
+      <c r="L15" s="2">
+        <f>bom[[#This Row],[Qty]]*bom[[#This Row],[Price]]</f>
+        <v>5.3100000000000001E-2</v>
       </c>
       <c r="N15" t="s">
+        <v>14</v>
+      </c>
+      <c r="O15" t="s">
         <v>91</v>
       </c>
-      <c r="O15">
+      <c r="P15">
         <v>3127309</v>
       </c>
-      <c r="P15" t="s">
+      <c r="Q15" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1761,20 +1871,27 @@
       <c r="I16">
         <v>300</v>
       </c>
-      <c r="M16" t="s">
-        <v>14</v>
+      <c r="K16" s="2">
+        <v>7.7600000000000002E-2</v>
+      </c>
+      <c r="L16" s="2">
+        <f>bom[[#This Row],[Qty]]*bom[[#This Row],[Price]]</f>
+        <v>0.23280000000000001</v>
       </c>
       <c r="N16" t="s">
+        <v>14</v>
+      </c>
+      <c r="O16" t="s">
         <v>97</v>
       </c>
-      <c r="O16">
+      <c r="P16">
         <v>3127351</v>
       </c>
-      <c r="P16" t="s">
+      <c r="Q16" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1803,17 +1920,24 @@
       <c r="I17">
         <v>200</v>
       </c>
-      <c r="M17" t="s">
-        <v>14</v>
+      <c r="K17" s="2">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="L17" s="2">
+        <f>bom[[#This Row],[Qty]]*bom[[#This Row],[Price]]</f>
+        <v>1E-3</v>
       </c>
       <c r="N17" t="s">
         <v>14</v>
       </c>
-      <c r="P17" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="O17" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1842,17 +1966,24 @@
       <c r="I18">
         <v>100</v>
       </c>
-      <c r="M18" t="s">
-        <v>14</v>
+      <c r="K18" s="2">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="L18" s="2">
+        <f>bom[[#This Row],[Qty]]*bom[[#This Row],[Price]]</f>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="N18" t="s">
         <v>14</v>
       </c>
-      <c r="P18" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="O18" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1881,17 +2012,24 @@
       <c r="I19">
         <v>500</v>
       </c>
-      <c r="M19" t="s">
-        <v>14</v>
+      <c r="K19" s="2">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="L19" s="2">
+        <f>bom[[#This Row],[Qty]]*bom[[#This Row],[Price]]</f>
+        <v>2.5000000000000001E-3</v>
       </c>
       <c r="N19" t="s">
         <v>14</v>
       </c>
-      <c r="P19" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="O19" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1920,17 +2058,24 @@
       <c r="I20">
         <v>200</v>
       </c>
-      <c r="M20" t="s">
-        <v>14</v>
+      <c r="K20" s="2">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="L20" s="2">
+        <f>bom[[#This Row],[Qty]]*bom[[#This Row],[Price]]</f>
+        <v>1E-3</v>
       </c>
       <c r="N20" t="s">
         <v>14</v>
       </c>
-      <c r="P20" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="O20" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1959,17 +2104,24 @@
       <c r="I21">
         <v>300</v>
       </c>
-      <c r="M21" t="s">
-        <v>14</v>
+      <c r="K21" s="2">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="L21" s="2">
+        <f>bom[[#This Row],[Qty]]*bom[[#This Row],[Price]]</f>
+        <v>1.5E-3</v>
       </c>
       <c r="N21" t="s">
         <v>14</v>
       </c>
-      <c r="P21" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="O21" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1998,17 +2150,24 @@
       <c r="I22">
         <v>200</v>
       </c>
-      <c r="M22" t="s">
-        <v>14</v>
+      <c r="K22" s="2">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="L22" s="2">
+        <f>bom[[#This Row],[Qty]]*bom[[#This Row],[Price]]</f>
+        <v>1E-3</v>
       </c>
       <c r="N22" t="s">
         <v>14</v>
       </c>
-      <c r="P22" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="O22" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2037,17 +2196,24 @@
       <c r="I23">
         <v>400</v>
       </c>
-      <c r="M23" t="s">
-        <v>14</v>
+      <c r="K23" s="2">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="L23" s="2">
+        <f>bom[[#This Row],[Qty]]*bom[[#This Row],[Price]]</f>
+        <v>2E-3</v>
       </c>
       <c r="N23" t="s">
         <v>14</v>
       </c>
-      <c r="P23" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="O23" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2076,17 +2242,24 @@
       <c r="I24">
         <v>200</v>
       </c>
-      <c r="M24" t="s">
-        <v>14</v>
+      <c r="K24" s="2">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="L24" s="2">
+        <f>bom[[#This Row],[Qty]]*bom[[#This Row],[Price]]</f>
+        <v>1E-3</v>
       </c>
       <c r="N24" t="s">
         <v>14</v>
       </c>
-      <c r="P24" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="O24" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2115,17 +2288,24 @@
       <c r="I25">
         <v>300</v>
       </c>
-      <c r="M25" t="s">
-        <v>14</v>
+      <c r="K25" s="2">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="L25" s="2">
+        <f>bom[[#This Row],[Qty]]*bom[[#This Row],[Price]]</f>
+        <v>1.5E-3</v>
       </c>
       <c r="N25" t="s">
         <v>14</v>
       </c>
-      <c r="P25" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="O25" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2154,17 +2334,24 @@
       <c r="I26">
         <v>300</v>
       </c>
-      <c r="M26" t="s">
-        <v>14</v>
+      <c r="K26" s="2">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="L26" s="2">
+        <f>bom[[#This Row],[Qty]]*bom[[#This Row],[Price]]</f>
+        <v>1.5E-3</v>
       </c>
       <c r="N26" t="s">
         <v>14</v>
       </c>
-      <c r="P26" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="O26" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2196,17 +2383,24 @@
       <c r="J27">
         <v>200</v>
       </c>
-      <c r="M27" t="s">
-        <v>14</v>
+      <c r="K27" s="2">
+        <v>6.4500000000000002E-2</v>
+      </c>
+      <c r="L27" s="2">
+        <f>bom[[#This Row],[Qty]]*bom[[#This Row],[Price]]</f>
+        <v>0.19350000000000001</v>
       </c>
       <c r="N27" t="s">
         <v>14</v>
       </c>
-      <c r="P27" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="O27" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>27</v>
       </c>
@@ -2236,19 +2430,23 @@
         <v>300</v>
       </c>
       <c r="K28" s="2">
-        <v>45337</v>
-      </c>
-      <c r="M28" t="s">
-        <v>14</v>
+        <v>7.6499999999999999E-2</v>
+      </c>
+      <c r="L28" s="2">
+        <f>bom[[#This Row],[Qty]]*bom[[#This Row],[Price]]</f>
+        <v>7.6499999999999999E-2</v>
       </c>
       <c r="N28" t="s">
         <v>14</v>
       </c>
-      <c r="P28" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="O28" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>28</v>
       </c>
@@ -2278,19 +2476,23 @@
         <v>400</v>
       </c>
       <c r="K29" s="2">
-        <v>45376</v>
-      </c>
-      <c r="M29" t="s">
-        <v>14</v>
+        <v>5.7200000000000001E-2</v>
+      </c>
+      <c r="L29" s="2">
+        <f>bom[[#This Row],[Qty]]*bom[[#This Row],[Price]]</f>
+        <v>5.7200000000000001E-2</v>
       </c>
       <c r="N29" t="s">
         <v>14</v>
       </c>
-      <c r="P29" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="O29" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2322,20 +2524,27 @@
       <c r="J30">
         <v>100</v>
       </c>
-      <c r="M30" t="s">
-        <v>14</v>
+      <c r="K30" s="2">
+        <v>0.35249999999999998</v>
+      </c>
+      <c r="L30" s="2">
+        <f>bom[[#This Row],[Qty]]*bom[[#This Row],[Price]]</f>
+        <v>0.70499999999999996</v>
       </c>
       <c r="N30" t="s">
+        <v>14</v>
+      </c>
+      <c r="O30" t="s">
         <v>155</v>
       </c>
-      <c r="O30">
+      <c r="P30">
         <v>1824861</v>
       </c>
-      <c r="P30" t="s">
+      <c r="Q30" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2367,20 +2576,27 @@
       <c r="J31">
         <v>50</v>
       </c>
-      <c r="M31" t="s">
-        <v>14</v>
+      <c r="K31" s="2">
+        <v>8.2400000000000001E-2</v>
+      </c>
+      <c r="L31" s="2">
+        <f>bom[[#This Row],[Qty]]*bom[[#This Row],[Price]]</f>
+        <v>8.2400000000000001E-2</v>
       </c>
       <c r="N31" t="s">
+        <v>14</v>
+      </c>
+      <c r="O31" t="s">
         <v>161</v>
       </c>
-      <c r="O31">
+      <c r="P31">
         <v>1827607</v>
       </c>
-      <c r="P31" t="s">
+      <c r="Q31" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>31</v>
       </c>
@@ -2412,20 +2628,27 @@
       <c r="J32">
         <v>1600</v>
       </c>
-      <c r="M32" t="s">
-        <v>14</v>
+      <c r="K32" s="2">
+        <v>5.21E-2</v>
+      </c>
+      <c r="L32" s="2">
+        <f>bom[[#This Row],[Qty]]*bom[[#This Row],[Price]]</f>
+        <v>1.6672</v>
       </c>
       <c r="N32" t="s">
+        <v>14</v>
+      </c>
+      <c r="O32" t="s">
         <v>167</v>
       </c>
-      <c r="O32">
+      <c r="P32">
         <v>2777317</v>
       </c>
-      <c r="P32" t="s">
+      <c r="Q32" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>32</v>
       </c>
@@ -2457,20 +2680,27 @@
       <c r="J33">
         <v>50</v>
       </c>
-      <c r="M33" t="s">
-        <v>14</v>
+      <c r="K33" s="2">
+        <v>0.15240000000000001</v>
+      </c>
+      <c r="L33" s="2">
+        <f>bom[[#This Row],[Qty]]*bom[[#This Row],[Price]]</f>
+        <v>0.15240000000000001</v>
       </c>
       <c r="N33" t="s">
+        <v>14</v>
+      </c>
+      <c r="O33" t="s">
         <v>174</v>
       </c>
-      <c r="O33">
+      <c r="P33">
         <v>3482799</v>
       </c>
-      <c r="P33" t="s">
+      <c r="Q33" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>33</v>
       </c>
@@ -2502,20 +2732,27 @@
       <c r="J34">
         <v>50</v>
       </c>
-      <c r="M34" t="s">
-        <v>14</v>
+      <c r="K34" s="2">
+        <v>1.0245</v>
+      </c>
+      <c r="L34" s="2">
+        <f>bom[[#This Row],[Qty]]*bom[[#This Row],[Price]]</f>
+        <v>1.0245</v>
       </c>
       <c r="N34" t="s">
+        <v>14</v>
+      </c>
+      <c r="O34" t="s">
         <v>179</v>
       </c>
-      <c r="O34">
+      <c r="P34">
         <v>2857611</v>
       </c>
-      <c r="P34" t="s">
+      <c r="Q34" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>34</v>
       </c>
@@ -2547,20 +2784,27 @@
       <c r="J35">
         <v>50</v>
       </c>
-      <c r="L35">
+      <c r="K35" s="2">
+        <v>1.542</v>
+      </c>
+      <c r="L35" s="2">
+        <f>bom[[#This Row],[Qty]]*bom[[#This Row],[Price]]</f>
+        <v>1.542</v>
+      </c>
+      <c r="M35">
         <v>1005004329064488</v>
       </c>
-      <c r="M35" t="s">
-        <v>14</v>
-      </c>
       <c r="N35" t="s">
         <v>14</v>
       </c>
-      <c r="P35" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="O35" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q35" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>35</v>
       </c>
@@ -2586,20 +2830,20 @@
         <f>50*bom[[#This Row],[Qty]]</f>
         <v>50</v>
       </c>
-      <c r="L36">
+      <c r="M36">
         <v>1005005036714708</v>
       </c>
-      <c r="M36" t="s">
-        <v>14</v>
-      </c>
       <c r="N36" t="s">
         <v>14</v>
       </c>
-      <c r="P36" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="O36" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>36</v>
       </c>
@@ -2631,17 +2875,24 @@
       <c r="J37">
         <v>50</v>
       </c>
-      <c r="M37" t="s">
-        <v>14</v>
+      <c r="K37" s="2">
+        <v>0.1923</v>
+      </c>
+      <c r="L37" s="2">
+        <f>bom[[#This Row],[Qty]]*bom[[#This Row],[Price]]</f>
+        <v>0.1923</v>
       </c>
       <c r="N37" t="s">
         <v>14</v>
       </c>
-      <c r="P37" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="O37" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q37" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>37</v>
       </c>
@@ -2673,13 +2924,20 @@
       <c r="J38">
         <v>50</v>
       </c>
-      <c r="M38" t="s">
-        <v>14</v>
+      <c r="K38" s="2">
+        <v>0.1037</v>
+      </c>
+      <c r="L38" s="2">
+        <f>bom[[#This Row],[Qty]]*bom[[#This Row],[Price]]</f>
+        <v>0.1037</v>
       </c>
       <c r="N38" t="s">
         <v>14</v>
       </c>
-      <c r="P38" t="s">
+      <c r="O38" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q38" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>